<commit_message>
Added Cards to ToDo list
</commit_message>
<xml_diff>
--- a/db/database_plan.xlsx
+++ b/db/database_plan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
   <si>
     <t>string</t>
   </si>
@@ -50,9 +50,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>comment</t>
-  </si>
-  <si>
     <t>Card</t>
   </si>
   <si>
@@ -63,6 +60,24 @@
   </si>
   <si>
     <t>board_id</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>duedate</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>to_do_id</t>
   </si>
 </sst>
 </file>
@@ -120,7 +135,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -128,79 +143,29 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -483,33 +448,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="5" width="17.140625" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B1" s="5"/>
+      <c r="D1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="G1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="5"/>
+      <c r="J1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="5"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -522,211 +498,144 @@
       <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>5</v>
       </c>
       <c r="E4" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H5" s="3" t="s">
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="K5" s="3" t="s">
+      <c r="C23" s="4"/>
+      <c r="E23" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="3"/>
-      <c r="N5" s="3" t="s">
+      <c r="F23" s="4"/>
+      <c r="H23" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="3"/>
-    </row>
-    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H7" s="6" t="s">
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="7"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="6"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="7"/>
-      <c r="K7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="L7" s="7"/>
-      <c r="N7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="O7" s="7"/>
-    </row>
-    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="9"/>
-      <c r="K8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="L8" s="9"/>
-      <c r="N8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="O8" s="9"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" t="s">
-        <v>3</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="7"/>
-      <c r="K9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="L9" s="7"/>
-      <c r="N9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="O9" s="7"/>
-    </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" s="9"/>
-      <c r="K10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="L10" s="9"/>
-      <c r="N10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="O10" s="9"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="H11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I11" s="7"/>
-      <c r="K11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="L11" s="7"/>
-      <c r="N11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="O11" s="7"/>
-    </row>
-    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H12" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="9"/>
-      <c r="K12" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="L12" s="9"/>
-      <c r="N12" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="O12" s="9"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" t="s">
-        <v>2</v>
-      </c>
+      <c r="C29" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="H3:O4"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
+  <mergeCells count="13">
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B21:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="E23:F23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>